<commit_message>
changes made in download.xlsx
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -1,29 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOMESH CHATTERJEE\Downloads\Gitdemo2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE966D-2A87-47C3-9C59-3A595D3D6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+  <si>
+    <t>sno</t>
+  </si>
+  <si>
+    <t>fruit_name</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>Papaya</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Kivi</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>newest</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -42,80 +113,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -440,182 +452,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sno</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>fruit_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>color</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>season</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Mango</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yellow</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>299</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Summer</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Apple</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>500</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Winter</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Papaya</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>187</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Banana</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Yellow</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>69</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Kivi</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
         <v>399</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Winter</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Orange</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
         <v>199</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Summer</t>
-        </is>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made in download
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOMESH CHATTERJEE\Downloads\Gitdemo2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOMESH CHATTERJEE\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE966D-2A87-47C3-9C59-3A595D3D6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46175743-7193-4062-B74D-DC55262B69D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>sno</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>newest</t>
+  </si>
+  <si>
+    <t>newest 2</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -461,7 +464,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +483,11 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -498,7 +504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -515,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -532,7 +538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -549,7 +555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
changes in download on 3-1-24
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOMESH CHATTERJEE\Downloads\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOMESH CHATTERJEE\Downloads\Gitdemo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46175743-7193-4062-B74D-DC55262B69D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB3F5D-B604-4DEA-9ECA-0F475020C7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>sno</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>newest 2</t>
+  </si>
+  <si>
+    <t>newest 3</t>
   </si>
 </sst>
 </file>
@@ -456,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,8 +489,11 @@
       <c r="G1" t="s">
         <v>19</v>
       </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -504,7 +510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -521,7 +527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -538,7 +544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -555,7 +561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -572,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>